<commit_message>
add a new script
</commit_message>
<xml_diff>
--- a/Automation with python/transactions2.xlsx
+++ b/Automation with python/transactions2.xlsx
@@ -1,33 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Automation with python\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DC3863-1AEE-427A-91A7-8A7E3E7FBB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="2880" yWindow="2880" windowWidth="19200" windowHeight="11170" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>transaction_id</t>
+  </si>
+  <si>
+    <t>product_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00;[Red]\-[$$-C09]#,##0.00"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,194 +68,234 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <spPr>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
             <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'Sheet1'!$B$2:$B$4</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <spPr>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F31D-4C67-A1D6-83E31F689357}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
             <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'Sheet1'!$C$2:$C$4</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <spPr>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-C09]#,##0.00;[Red]\-[$$-C09]#,##0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F31D-4C67-A1D6-83E31F689357}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
             <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'Sheet1'!$D$2:$D$4</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.3550000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1550000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F31D-4C67-A1D6-83E31F689357}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="10"/>
+        <c:axId val="100"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="10"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="100"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="10"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="1"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>1</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5400000" cy="2700000"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -552,92 +614,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="11.54296875" customWidth="1" min="1" max="1025"/>
+    <col min="1" max="1025" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>transaction_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>product_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">price </t>
-        </is>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1001</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="1">
         <v>5.95</v>
       </c>
-      <c r="D2" t="n">
-        <v>5.355</v>
+      <c r="D2">
+        <v>5.3550000000000004</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1002</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="1">
         <v>6.95</v>
       </c>
-      <c r="D3" t="n">
-        <v>6.255</v>
+      <c r="D3">
+        <v>6.2549999999999999</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>1003</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="1">
         <v>7.95</v>
       </c>
-      <c r="D4" t="n">
-        <v>7.155</v>
+      <c r="D4">
+        <v>7.1550000000000002</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" paperSize="9" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A3C4D0-52CC-46B5-BBAE-1CFCEB1C4803}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3132FC19-51D0-466C-9874-6A48764020C2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>